<commit_message>
add step by step MLP
</commit_message>
<xml_diff>
--- a/step_by_step_cnns.xlsx
+++ b/step_by_step_cnns.xlsx
@@ -490,8 +490,8 @@
   </sheetPr>
   <dimension ref="A1:AU74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,7 +499,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="1" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="1" width="8.67"/>
@@ -1891,7 +1893,7 @@
       </c>
       <c r="R13" s="5" t="n">
         <f aca="false">$O$43*(N13+N18*$P$43)*1+$O$43*$Q$43*A13</f>
-        <v>-0.00075329892467932</v>
+        <v>-0.000753298924679321</v>
       </c>
       <c r="S13" s="5" t="n">
         <f aca="false">$O$43*(O13+O18*$P$43)*1+$O$43*$Q$43*B13</f>
@@ -1899,7 +1901,7 @@
       </c>
       <c r="T13" s="5" t="n">
         <f aca="false">$O$43*(P13+P18*$P$43)*1+$O$43*$Q$43*C13</f>
-        <v>0.000736008869092887</v>
+        <v>0.000736008869092888</v>
       </c>
       <c r="Z13" s="1" t="n">
         <f aca="false">A6*Q30</f>
@@ -2010,7 +2012,7 @@
       </c>
       <c r="N14" s="8" t="n">
         <f aca="false">SUM(Z10:AE16)</f>
-        <v>0.0129620101108045</v>
+        <v>0.0129620101108044</v>
       </c>
       <c r="O14" s="8" t="n">
         <f aca="false">SUM(AH10:AM16)</f>
@@ -2022,7 +2024,7 @@
       </c>
       <c r="R14" s="5" t="n">
         <f aca="false">$O$43*(N14+N19*$P$43)*1+$O$43*$Q$43*A14</f>
-        <v>0.000134025191988495</v>
+        <v>0.000134025191988494</v>
       </c>
       <c r="S14" s="5" t="n">
         <f aca="false">$O$43*(O14+O19*$P$43)*1+$O$43*$Q$43*B14</f>
@@ -4576,8 +4578,8 @@
         <v>4.81428432870336E-005</v>
       </c>
       <c r="C74" s="22" t="n">
-        <f aca="false">$O$43*(M$59+M$61*$P$43)*$E52+$O$43*$Q$43*C52</f>
-        <v>-0.000352934802080236</v>
+        <f aca="false">$O$43*(M$59+M$61*$P$43)*$E52</f>
+        <v>-0.000348729338313975</v>
       </c>
       <c r="E74" s="9" t="n">
         <f aca="false">A52-A74</f>
@@ -4589,7 +4591,7 @@
       </c>
       <c r="G74" s="9" t="n">
         <f aca="false">C52-C74</f>
-        <v>-0.420193441824048</v>
+        <v>-0.420197647287814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update todo && change default activation func for FC layer
</commit_message>
<xml_diff>
--- a/step_by_step_cnns.xlsx
+++ b/step_by_step_cnns.xlsx
@@ -399,15 +399,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,7 +491,7 @@
   <dimension ref="A1:AU74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+      <selection pane="topLeft" activeCell="U48" activeCellId="0" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="O3" s="5" t="n">
         <f aca="false">$I$13*R26+$J$13*S26+$K$13*T26+$I$14*R27+$J$14*S27+$K$14*T27+$I$15*R28+$J$15*S28+$K$15*T28</f>
-        <v>-0.0143638128937038</v>
+        <v>-0.15247144445936</v>
       </c>
       <c r="P3" s="5" t="n">
         <f aca="false">$I$13*S26+$J$13*T26+$K$13*U26+$I$14*S27+$J$14*T27+$K$14*U27+$I$15*S28+$J$15*T28+$K$15*U28</f>
@@ -758,7 +758,7 @@
       </c>
       <c r="AA3" s="1" t="n">
         <f aca="false">B3*R28</f>
-        <v>-0.00330686857057358</v>
+        <v>-0.0351023110175448</v>
       </c>
       <c r="AB3" s="1" t="n">
         <f aca="false">C3*S28</f>
@@ -782,7 +782,7 @@
       </c>
       <c r="AI3" s="1" t="n">
         <f aca="false">C3*R28</f>
-        <v>0.00363755542763093</v>
+        <v>0.0386125421192993</v>
       </c>
       <c r="AJ3" s="1" t="n">
         <f aca="false">D3*S28</f>
@@ -806,7 +806,7 @@
       </c>
       <c r="AQ3" s="1" t="n">
         <f aca="false">D3*R28</f>
-        <v>0.00396824228468829</v>
+        <v>0.0421227732210537</v>
       </c>
       <c r="AR3" s="1" t="n">
         <f aca="false">E3*S28</f>
@@ -852,15 +852,15 @@
       </c>
       <c r="M4" s="5" t="n">
         <f aca="false">$I$13*P27+$J$13*Q27+$K$13*R27+$I$14*P28+$J$14*Q28+$K$14*R28+$I$15*P29+$J$15*Q29+$K$15*R29</f>
-        <v>0.0130294890707744</v>
+        <v>0.17210728235516</v>
       </c>
       <c r="N4" s="5" t="n">
         <f aca="false">$I$13*Q27+$J$13*R27+$K$13*S27+$I$14*Q28+$J$14*R28+$K$14*S28+$I$15*Q29+$J$15*R29+$K$15*S29</f>
-        <v>-0.00157709613006276</v>
+        <v>-0.0368557966755346</v>
       </c>
       <c r="O4" s="5" t="n">
         <f aca="false">$I$13*R27+$J$13*S27+$K$13*T27+$I$14*R28+$J$14*S28+$K$14*T28+$I$15*R29+$J$15*S29+$K$15*T29</f>
-        <v>-0.00497721689020475</v>
+        <v>-0.193108895394413</v>
       </c>
       <c r="P4" s="5" t="n">
         <f aca="false">$I$13*S27+$J$13*T27+$K$13*U27+$I$14*S28+$J$14*T28+$K$14*U28+$I$15*S29+$J$15*T29+$K$15*U29</f>
@@ -888,7 +888,7 @@
       </c>
       <c r="AA4" s="1" t="n">
         <f aca="false">B4*R29</f>
-        <v>-0.00264438554066516</v>
+        <v>0.0300602478586864</v>
       </c>
       <c r="AB4" s="1" t="n">
         <f aca="false">C4*S29</f>
@@ -912,7 +912,7 @@
       </c>
       <c r="AI4" s="1" t="n">
         <f aca="false">C4*R29</f>
-        <v>0.00279129584847989</v>
+        <v>-0.0317302616286135</v>
       </c>
       <c r="AJ4" s="1" t="n">
         <f aca="false">D4*S29</f>
@@ -936,7 +936,7 @@
       </c>
       <c r="AQ4" s="1" t="n">
         <f aca="false">D4*R29</f>
-        <v>-0.00293820615629462</v>
+        <v>0.0334002753985405</v>
       </c>
       <c r="AR4" s="1" t="n">
         <f aca="false">E4*S29</f>
@@ -982,23 +982,23 @@
       </c>
       <c r="M5" s="5" t="n">
         <f aca="false">$I$13*P28+$J$13*Q28+$K$13*R28+$I$14*P29+$J$14*Q29+$K$14*R29+$I$15*P30+$J$15*Q30+$K$15*R30</f>
-        <v>-0.00102974789238652</v>
+        <v>0.131330005972708</v>
       </c>
       <c r="N5" s="5" t="n">
         <f aca="false">$I$13*Q28+$J$13*R28+$K$13*S28+$I$14*Q29+$J$14*R29+$K$14*S29+$I$15*Q30+$J$15*R30+$K$15*S30</f>
-        <v>0.00728514632951709</v>
+        <v>0.0529935743276317</v>
       </c>
       <c r="O5" s="5" t="n">
         <f aca="false">$I$13*R28+$J$13*S28+$K$13*T28+$I$14*R29+$J$14*S29+$K$14*T29+$I$15*R30+$J$15*S30+$K$15*T30</f>
-        <v>-0.00239628009668513</v>
+        <v>-0.141241454097748</v>
       </c>
       <c r="P5" s="5" t="n">
         <f aca="false">$I$13*S28+$J$13*T28+$K$13*U28+$I$14*S29+$J$14*T29+$K$14*U29+$I$15*S30+$J$15*T30+$K$15*U30</f>
-        <v>-0.00350249432877462</v>
+        <v>-0.0342751447325266</v>
       </c>
       <c r="Q5" s="5" t="n">
         <f aca="false">$I$13*T28+$J$13*U28+$K$13*V28+$I$14*T29+$J$14*U29+$K$14*V29+$I$15*T30+$J$15*U30+$K$15*V30</f>
-        <v>-0.024425367641705</v>
+        <v>-0.23902480132138</v>
       </c>
       <c r="R5" s="5" t="n">
         <f aca="false">$I$13*U28+$J$13*V28+$K$13*W28+$I$14*U29+$J$14*V29+$K$14*W29+$I$15*U30+$J$15*V30+$K$15*W30</f>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="AC5" s="1" t="n">
         <f aca="false">D5*T30</f>
-        <v>-0.0157451330851364</v>
+        <v>-0.154080682127686</v>
       </c>
       <c r="AD5" s="1" t="n">
         <f aca="false">E5*U30</f>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="AK5" s="1" t="n">
         <f aca="false">E5*T30</f>
-        <v>0.0163074592667484</v>
+        <v>0.159583563632246</v>
       </c>
       <c r="AL5" s="1" t="n">
         <f aca="false">F5*U30</f>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="AS5" s="1" t="n">
         <f aca="false">F5*T30</f>
-        <v>0.0168697854483605</v>
+        <v>0.165086445136807</v>
       </c>
       <c r="AT5" s="1" t="n">
         <f aca="false">G5*U30</f>
@@ -1112,23 +1112,23 @@
       </c>
       <c r="M6" s="5" t="n">
         <f aca="false">$I$13*P29+$J$13*Q29+$K$13*R29+$I$14*P30+$J$14*Q30+$K$14*R30+$I$15*P31+$J$15*Q31+$K$15*R31</f>
-        <v>-0.00241755680723369</v>
+        <v>0.0274817554854802</v>
       </c>
       <c r="N6" s="5" t="n">
         <f aca="false">$I$13*Q29+$J$13*R29+$K$13*S29+$I$14*Q30+$J$14*R30+$K$14*S30+$I$15*Q31+$J$15*R31+$K$15*S31</f>
-        <v>-0.00274462351418009</v>
+        <v>0.0311997104228152</v>
       </c>
       <c r="O6" s="5" t="n">
         <f aca="false">$I$13*R29+$J$13*S29+$K$13*T29+$I$14*R30+$J$14*S30+$K$14*T30+$I$15*R31+$J$15*S31+$K$15*T31</f>
-        <v>0.0306919125480735</v>
+        <v>0.175100286008046</v>
       </c>
       <c r="P6" s="5" t="n">
         <f aca="false">$I$13*S29+$J$13*T29+$K$13*U29+$I$14*S30+$J$14*T30+$K$14*U30+$I$15*S31+$J$15*T31+$K$15*U31</f>
-        <v>-0.00423783085086395</v>
+        <v>-0.0414710923503897</v>
       </c>
       <c r="Q6" s="5" t="n">
         <f aca="false">$I$13*T29+$J$13*U29+$K$13*V29+$I$14*T30+$J$14*U30+$K$14*V30+$I$15*T31+$J$15*U31+$K$15*V31</f>
-        <v>-0.0193148215943359</v>
+        <v>-0.189013384030348</v>
       </c>
       <c r="R6" s="5" t="n">
         <f aca="false">$I$13*U29+$J$13*V29+$K$13*W29+$I$14*U30+$J$14*V30+$K$14*W30+$I$15*U31+$J$15*V31+$K$15*W31</f>
@@ -1250,23 +1250,23 @@
       </c>
       <c r="O7" s="5" t="n">
         <f aca="false">$I$13*R30+$J$13*S30+$K$13*T30+$I$14*R31+$J$14*S31+$K$14*T31+$I$15*R32+$J$15*S32+$K$15*T32</f>
-        <v>0.00193329508557937</v>
+        <v>0.0550818925711669</v>
       </c>
       <c r="P7" s="5" t="n">
         <f aca="false">$I$13*S30+$J$13*T30+$K$13*U30+$I$14*S31+$J$14*T31+$K$14*U31+$I$15*S32+$J$15*T32+$K$15*U32</f>
-        <v>0.014862062489866</v>
+        <v>0.123917674688608</v>
       </c>
       <c r="Q7" s="5" t="n">
         <f aca="false">$I$13*T30+$J$13*U30+$K$13*V30+$I$14*T31+$J$14*U31+$K$14*V31+$I$15*T32+$J$15*U32+$K$15*V32</f>
-        <v>0.0129421398643107</v>
+        <v>-0.0257455533687688</v>
       </c>
       <c r="R7" s="5" t="n">
         <f aca="false">$I$13*U30+$J$13*V30+$K$13*W30+$I$14*U31+$J$14*V31+$K$14*W31+$I$15*U32+$J$15*V32+$K$15*W32</f>
-        <v>-0.00310926098765267</v>
+        <v>-0.0290505858196268</v>
       </c>
       <c r="S7" s="5" t="n">
         <f aca="false">$I$13*V30+$J$13*W30+$K$13*X30+$I$14*V31+$J$14*W31+$K$14*X31+$I$15*V32+$J$15*W32+$K$15*X32</f>
-        <v>-0.0216830737150679</v>
+        <v>-0.20259026060994</v>
       </c>
       <c r="T7" s="5" t="n">
         <f aca="false">$I$13*W30+$J$13*X30+$K$13*Y30+$I$14*W31+$J$14*X31+$K$14*Y31+$I$15*W32+$J$15*X32+$K$15*Y32</f>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="AC7" s="1" t="n">
         <f aca="false">D7*T32</f>
-        <v>-0.0307753111031962</v>
+        <v>-0.149133586318115</v>
       </c>
       <c r="AD7" s="1" t="n">
         <f aca="false">E7*U32</f>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="AE7" s="1" t="n">
         <f aca="false">F7*V32</f>
-        <v>-0.0229628544563403</v>
+        <v>-0.214547565063403</v>
       </c>
       <c r="AH7" s="1" t="n">
         <f aca="false">B7*Q32</f>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="AK7" s="1" t="n">
         <f aca="false">E7*T32</f>
-        <v>-0.0314747499919052</v>
+        <v>-0.152522986007163</v>
       </c>
       <c r="AL7" s="1" t="n">
         <f aca="false">F7*U32</f>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="AM7" s="1" t="n">
         <f aca="false">G7*V32</f>
-        <v>0.0234620469445216</v>
+        <v>0.219211642564782</v>
       </c>
       <c r="AP7" s="1" t="n">
         <f aca="false">C7*Q32</f>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="AS7" s="1" t="n">
         <f aca="false">F7*T32</f>
-        <v>0.0321741888806142</v>
+        <v>0.155912385696211</v>
       </c>
       <c r="AT7" s="1" t="n">
         <f aca="false">G7*U32</f>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="AU7" s="1" t="n">
         <f aca="false">H7*V32</f>
-        <v>0.0239612394327029</v>
+        <v>0.22387572006616</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,23 +1380,23 @@
       </c>
       <c r="O8" s="5" t="n">
         <f aca="false">$I$13*R31+$J$13*S31+$K$13*T31+$I$14*R32+$J$14*S32+$K$14*T32+$I$15*R33+$J$15*S33+$K$15*T33</f>
-        <v>-0.030810918700842</v>
+        <v>-0.149306136604261</v>
       </c>
       <c r="P8" s="5" t="n">
         <f aca="false">$I$13*S31+$J$13*T31+$K$13*U31+$I$14*S32+$J$14*T32+$K$14*U32+$I$15*S33+$J$15*T33+$K$15*U33</f>
-        <v>0.00527114652988031</v>
+        <v>0.0255433643992536</v>
       </c>
       <c r="Q8" s="5" t="n">
         <f aca="false">$I$13*T31+$J$13*U31+$K$13*V31+$I$14*T32+$J$14*U32+$K$14*V32+$I$15*T33+$J$15*U33+$K$15*V33</f>
-        <v>0.0460142618490307</v>
+        <v>0.32187620579061</v>
       </c>
       <c r="R8" s="5" t="n">
         <f aca="false">$I$13*U31+$J$13*V31+$K$13*W31+$I$14*U32+$J$14*V32+$K$14*W32+$I$15*U33+$J$15*V33+$K$15*W33</f>
-        <v>-0.00376203953525661</v>
+        <v>-0.0351496554357469</v>
       </c>
       <c r="S8" s="5" t="n">
         <f aca="false">$I$13*V31+$J$13*W31+$K$13*X31+$I$14*V32+$J$14*W32+$K$14*X32+$I$15*V33+$J$15*W33+$K$15*X33</f>
-        <v>-0.0171463007872309</v>
+        <v>-0.160202081615745</v>
       </c>
       <c r="T8" s="5" t="n">
         <f aca="false">$I$13*W31+$J$13*X31+$K$13*Y31+$I$14*W32+$J$14*X32+$K$14*Y32+$I$15*W33+$J$15*X33+$K$15*Y33</f>
@@ -1510,23 +1510,23 @@
       </c>
       <c r="O9" s="5" t="n">
         <f aca="false">$I$13*R32+$J$13*S32+$K$13*T32+$I$14*R33+$J$14*S33+$K$14*T33+$I$15*R34+$J$15*S34+$K$15*T34</f>
-        <v>-0.0115099700749035</v>
+        <v>-0.0557759793208483</v>
       </c>
       <c r="P9" s="5" t="n">
         <f aca="false">$I$13*S32+$J$13*T32+$K$13*U32+$I$14*S33+$J$14*T33+$K$14*U33+$I$15*S34+$J$15*T34+$K$15*U34</f>
-        <v>-0.0130671322471372</v>
+        <v>-0.0633218065082783</v>
       </c>
       <c r="Q9" s="5" t="n">
         <f aca="false">$I$13*T32+$J$13*U32+$K$13*V32+$I$14*T33+$J$14*U33+$K$14*V33+$I$15*T34+$J$15*U34+$K$15*V34</f>
-        <v>0.0364042334227695</v>
+        <v>0.213355222911012</v>
       </c>
       <c r="R9" s="5" t="n">
         <f aca="false">$I$13*U32+$J$13*V32+$K$13*W32+$I$14*U33+$J$14*V33+$K$14*W33+$I$15*U34+$J$15*V34+$K$15*W34</f>
-        <v>0.00932606745942103</v>
+        <v>0.0871357290897849</v>
       </c>
       <c r="S9" s="5" t="n">
         <f aca="false">$I$13*V32+$J$13*W32+$K$13*X32+$I$14*V33+$J$14*W33+$K$14*X33+$I$15*V34+$J$15*W34+$K$15*X34</f>
-        <v>-0.0201189788665989</v>
+        <v>-0.187976539920064</v>
       </c>
       <c r="T9" s="5" t="n">
         <f aca="false">$I$13*W32+$J$13*X32+$K$13*Y32+$I$14*W33+$J$14*X33+$K$14*Y33+$I$15*W34+$J$15*X34+$K$15*Y34</f>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="AA11" s="1" t="n">
         <f aca="false">B4*R28</f>
-        <v>0.00595236342703244</v>
+        <v>0.0631841598315806</v>
       </c>
       <c r="AB11" s="1" t="n">
         <f aca="false">C4*S28</f>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="AI11" s="1" t="n">
         <f aca="false">C4*R28</f>
-        <v>-0.0062830502840898</v>
+        <v>-0.0666943909333351</v>
       </c>
       <c r="AJ11" s="1" t="n">
         <f aca="false">D4*S28</f>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="AQ11" s="1" t="n">
         <f aca="false">D4*R28</f>
-        <v>0.00661373714114715</v>
+        <v>0.0702046220350896</v>
       </c>
       <c r="AR11" s="1" t="n">
         <f aca="false">E4*S28</f>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="AA12" s="1" t="n">
         <f aca="false">B5*R29</f>
-        <v>-0.00381966800318301</v>
+        <v>0.0434203580181026</v>
       </c>
       <c r="AB12" s="1" t="n">
         <f aca="false">C5*S29</f>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="AI12" s="1" t="n">
         <f aca="false">C5*R29</f>
-        <v>-0.00396657831099774</v>
+        <v>0.0450903717880297</v>
       </c>
       <c r="AJ12" s="1" t="n">
         <f aca="false">D5*S29</f>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="AQ12" s="1" t="n">
         <f aca="false">D5*R29</f>
-        <v>0.00411348861881247</v>
+        <v>-0.0467603855579567</v>
       </c>
       <c r="AR12" s="1" t="n">
         <f aca="false">E5*S29</f>
@@ -1881,27 +1881,27 @@
       </c>
       <c r="N13" s="8" t="n">
         <f aca="false">SUM(Z2:AE8)</f>
-        <v>-0.0754345527559117</v>
+        <v>-0.522803896668063</v>
       </c>
       <c r="O13" s="8" t="n">
         <f aca="false">SUM(AH2:AM8)</f>
-        <v>0.0147236074954756</v>
+        <v>0.233154500680551</v>
       </c>
       <c r="P13" s="8" t="n">
         <f aca="false">SUM(AP2:AU8)</f>
-        <v>0.0740352498900713</v>
+        <v>0.620397599518772</v>
       </c>
       <c r="R13" s="5" t="n">
         <f aca="false">$O$43*(N13+N18*$P$43)*1+$O$43*$Q$43*A13</f>
-        <v>-0.000753298924679321</v>
+        <v>-0.00522699236380083</v>
       </c>
       <c r="S13" s="5" t="n">
         <f aca="false">$O$43*(O13+O18*$P$43)*1+$O$43*$Q$43*B13</f>
-        <v>0.000146613216826626</v>
+        <v>0.00233092214867738</v>
       </c>
       <c r="T13" s="5" t="n">
         <f aca="false">$O$43*(P13+P18*$P$43)*1+$O$43*$Q$43*C13</f>
-        <v>0.000736008869092888</v>
+        <v>0.00619963236537989</v>
       </c>
       <c r="Z13" s="1" t="n">
         <f aca="false">A6*Q30</f>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="AC13" s="1" t="n">
         <f aca="false">D6*T30</f>
-        <v>0.0202437425380326</v>
+        <v>0.198103734164168</v>
       </c>
       <c r="AD13" s="1" t="n">
         <f aca="false">E6*U30</f>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="AK13" s="1" t="n">
         <f aca="false">E6*T30</f>
-        <v>-0.0208060687196446</v>
+        <v>-0.203606615668728</v>
       </c>
       <c r="AL13" s="1" t="n">
         <f aca="false">F6*U30</f>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="AS13" s="1" t="n">
         <f aca="false">F6*T30</f>
-        <v>0.0213683949012566</v>
+        <v>0.209109497173288</v>
       </c>
       <c r="AT13" s="1" t="n">
         <f aca="false">G6*U30</f>
@@ -2012,27 +2012,27 @@
       </c>
       <c r="N14" s="8" t="n">
         <f aca="false">SUM(Z10:AE16)</f>
-        <v>0.0129620101108044</v>
+        <v>0.380319653257782</v>
       </c>
       <c r="O14" s="8" t="n">
         <f aca="false">SUM(AH10:AM16)</f>
-        <v>-0.0955815452662814</v>
+        <v>-0.661373080909389</v>
       </c>
       <c r="P14" s="8" t="n">
         <f aca="false">SUM(AP10:AU16)</f>
-        <v>0.0222807000090833</v>
+        <v>0.310714490519013</v>
       </c>
       <c r="R14" s="5" t="n">
         <f aca="false">$O$43*(N14+N19*$P$43)*1+$O$43*$Q$43*A14</f>
-        <v>0.000134025191988494</v>
+        <v>0.00380760162345827</v>
       </c>
       <c r="S14" s="5" t="n">
         <f aca="false">$O$43*(O14+O19*$P$43)*1+$O$43*$Q$43*B14</f>
-        <v>-0.000956569077692101</v>
+        <v>-0.00661448443412318</v>
       </c>
       <c r="T14" s="5" t="n">
         <f aca="false">$O$43*(P14+P19*$P$43)*1+$O$43*$Q$43*C14</f>
-        <v>0.000219372192638161</v>
+        <v>0.00310371009773745</v>
       </c>
       <c r="Z14" s="1" t="n">
         <f aca="false">A7*Q31</f>
@@ -2143,27 +2143,27 @@
       </c>
       <c r="N15" s="8" t="n">
         <f aca="false">SUM(Z18:AE25)</f>
-        <v>0.01732886075342</v>
+        <v>0.475982086766358</v>
       </c>
       <c r="O15" s="8" t="n">
         <f aca="false">SUM(AH18:AM25)</f>
-        <v>0.017874717083747</v>
+        <v>0.48793989095493</v>
       </c>
       <c r="P15" s="8" t="n">
         <f aca="false">SUM(AP18:AU25)</f>
-        <v>-0.115728537776651</v>
+        <v>-0.799942265150716</v>
       </c>
       <c r="R15" s="5" t="n">
         <f aca="false">$O$43*(N15+N20*$P$43)*1+$O$43*$Q$43*A15</f>
-        <v>0.000174934208066385</v>
+        <v>0.00476146646819577</v>
       </c>
       <c r="S15" s="5" t="n">
         <f aca="false">$O$43*(O15+O20*$P$43)*1+$O$43*$Q$43*B15</f>
-        <v>0.000180615401566141</v>
+        <v>0.00488126714027797</v>
       </c>
       <c r="T15" s="5" t="n">
         <f aca="false">$O$43*(P15+P20*$P$43)*1+$O$43*$Q$43*C15</f>
-        <v>-0.00116131568257737</v>
+        <v>-0.00800345295631802</v>
       </c>
       <c r="Z15" s="1" t="n">
         <f aca="false">A8*Q32</f>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="AC15" s="1" t="n">
         <f aca="false">D8*T32</f>
-        <v>-0.0363708222128683</v>
+        <v>-0.176248783830499</v>
       </c>
       <c r="AD15" s="1" t="n">
         <f aca="false">E8*U32</f>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="AE15" s="1" t="n">
         <f aca="false">F8*V32</f>
-        <v>0.0269563943617907</v>
+        <v>0.25186018507443</v>
       </c>
       <c r="AH15" s="1" t="n">
         <f aca="false">B8*Q32</f>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="AK15" s="1" t="n">
         <f aca="false">E8*T32</f>
-        <v>-0.0370702611015773</v>
+        <v>-0.179638183519547</v>
       </c>
       <c r="AL15" s="1" t="n">
         <f aca="false">F8*U32</f>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AM15" s="1" t="n">
         <f aca="false">G8*V32</f>
-        <v>-0.0274555868499721</v>
+        <v>-0.256524262575808</v>
       </c>
       <c r="AP15" s="1" t="n">
         <f aca="false">C8*Q32</f>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="AS15" s="1" t="n">
         <f aca="false">F8*T32</f>
-        <v>-0.0377696999902863</v>
+        <v>-0.183027583208595</v>
       </c>
       <c r="AT15" s="1" t="n">
         <f aca="false">G8*U32</f>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="AU15" s="1" t="n">
         <f aca="false">H8*V32</f>
-        <v>0.0279547793381534</v>
+        <v>0.261188340077187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,15 +2369,15 @@
       </c>
       <c r="R18" s="9" t="n">
         <f aca="false">A13-R13</f>
-        <v>0.105413586904299</v>
+        <v>0.109887280343421</v>
       </c>
       <c r="S18" s="9" t="n">
         <f aca="false">B13-S13</f>
-        <v>-0.0624324260298464</v>
+        <v>-0.0646167349616972</v>
       </c>
       <c r="T18" s="9" t="n">
         <f aca="false">C13-T13</f>
-        <v>-0.435098989651617</v>
+        <v>-0.440562613147904</v>
       </c>
       <c r="Y18" s="6" t="s">
         <v>17</v>
@@ -2497,15 +2497,15 @@
       </c>
       <c r="R19" s="9" t="n">
         <f aca="false">A14-R14</f>
-        <v>0.440375062853023</v>
+        <v>0.436701486421554</v>
       </c>
       <c r="S19" s="9" t="n">
         <f aca="false">B14-S14</f>
-        <v>-0.0744059338510422</v>
+        <v>-0.0687480184946111</v>
       </c>
       <c r="T19" s="9" t="n">
         <f aca="false">C14-T14</f>
-        <v>-0.343700117459847</v>
+        <v>-0.346584455364946</v>
       </c>
       <c r="Z19" s="1" t="n">
         <f aca="false">A5*Q28</f>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="AA19" s="1" t="n">
         <f aca="false">B5*R28</f>
-        <v>0.0085978582834913</v>
+        <v>0.0912660086456164</v>
       </c>
       <c r="AB19" s="1" t="n">
         <f aca="false">C5*S28</f>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="AI19" s="1" t="n">
         <f aca="false">C5*R28</f>
-        <v>0.00892854514054866</v>
+        <v>0.0947762397473709</v>
       </c>
       <c r="AJ19" s="1" t="n">
         <f aca="false">D5*S28</f>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="AQ19" s="1" t="n">
         <f aca="false">D5*R28</f>
-        <v>-0.00925923199760602</v>
+        <v>-0.0982864708491254</v>
       </c>
       <c r="AR19" s="1" t="n">
         <f aca="false">E5*S28</f>
@@ -2616,15 +2616,15 @@
       </c>
       <c r="R20" s="9" t="n">
         <f aca="false">A15-R15</f>
-        <v>0.164385119010424</v>
+        <v>0.159798586750294</v>
       </c>
       <c r="S20" s="9" t="n">
         <f aca="false">B15-S15</f>
-        <v>0.186642457465543</v>
+        <v>0.181941805726831</v>
       </c>
       <c r="T20" s="9" t="n">
         <f aca="false">C15-T15</f>
-        <v>-0.401869165402938</v>
+        <v>-0.395027028129197</v>
       </c>
       <c r="Z20" s="1" t="n">
         <f aca="false">A6*Q29</f>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="AA20" s="1" t="n">
         <f aca="false">B6*R29</f>
-        <v>-0.00499495046570086</v>
+        <v>0.0567804681775188</v>
       </c>
       <c r="AB20" s="1" t="n">
         <f aca="false">C6*S29</f>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="AI20" s="1" t="n">
         <f aca="false">C6*R29</f>
-        <v>-0.00514186077351559</v>
+        <v>0.0584504819474459</v>
       </c>
       <c r="AJ20" s="1" t="n">
         <f aca="false">D6*S29</f>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="AQ20" s="1" t="n">
         <f aca="false">D6*R29</f>
-        <v>-0.00528877108133032</v>
+        <v>0.0601204957173729</v>
       </c>
       <c r="AR20" s="1" t="n">
         <f aca="false">E6*S29</f>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="AC21" s="1" t="n">
         <f aca="false">D7*T30</f>
-        <v>0.0247423519909287</v>
+        <v>0.24212678620065</v>
       </c>
       <c r="AD21" s="1" t="n">
         <f aca="false">E7*U30</f>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="AK21" s="1" t="n">
         <f aca="false">E7*T30</f>
-        <v>0.0253046781725407</v>
+        <v>0.24762966770521</v>
       </c>
       <c r="AL21" s="1" t="n">
         <f aca="false">F7*U30</f>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="AS21" s="1" t="n">
         <f aca="false">F7*T30</f>
-        <v>-0.0258670043541527</v>
+        <v>-0.25313254920977</v>
       </c>
       <c r="AT21" s="1" t="n">
         <f aca="false">G7*U30</f>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="AC23" s="1" t="n">
         <f aca="false">D9*T32</f>
-        <v>-0.0419663333225403</v>
+        <v>-0.203363981342884</v>
       </c>
       <c r="AD23" s="1" t="n">
         <f aca="false">E9*U32</f>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="AE23" s="1" t="n">
         <f aca="false">F9*V32</f>
-        <v>0.0309499342672412</v>
+        <v>0.289172805085457</v>
       </c>
       <c r="AH23" s="1" t="n">
         <f aca="false">B9*Q32</f>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="AK23" s="1" t="n">
         <f aca="false">E9*T32</f>
-        <v>-0.0426657722112493</v>
+        <v>-0.206753381031932</v>
       </c>
       <c r="AL23" s="1" t="n">
         <f aca="false">F9*U32</f>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="AM23" s="1" t="n">
         <f aca="false">G9*V32</f>
-        <v>0.0314491267554225</v>
+        <v>0.293836882586835</v>
       </c>
       <c r="AP23" s="1" t="n">
         <f aca="false">C9*Q32</f>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="AS23" s="1" t="n">
         <f aca="false">F9*T32</f>
-        <v>-0.0433652110999583</v>
+        <v>-0.21014278072098</v>
       </c>
       <c r="AT23" s="1" t="n">
         <f aca="false">G9*U32</f>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="AU23" s="1" t="n">
         <f aca="false">H9*V32</f>
-        <v>-0.0319483192436038</v>
+        <v>-0.298500960088213</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,19 +3153,19 @@
       </c>
       <c r="K27" s="11" t="n">
         <f aca="false">E56</f>
-        <v>-0.0498126796585316</v>
+        <v>-0.300902664233209</v>
       </c>
       <c r="L27" s="12" t="n">
         <f aca="false">E56</f>
-        <v>-0.0498126796585316</v>
+        <v>-0.300902664233209</v>
       </c>
       <c r="M27" s="11" t="n">
         <f aca="false">E57</f>
-        <v>-0.0191150997460902</v>
+        <v>-0.254969149404916</v>
       </c>
       <c r="N27" s="12" t="n">
         <f aca="false">E57</f>
-        <v>-0.0191150997460902</v>
+        <v>-0.254969149404916</v>
       </c>
       <c r="Q27" s="5" t="n">
         <f aca="false">IF(A18&lt;0,0,I27)</f>
@@ -3223,23 +3223,23 @@
       </c>
       <c r="J28" s="11" t="n">
         <f aca="false">E55</f>
-        <v>0.0330686857057358</v>
+        <v>0.351023110175448</v>
       </c>
       <c r="K28" s="12" t="n">
         <f aca="false">E56</f>
-        <v>-0.0498126796585316</v>
+        <v>-0.300902664233209</v>
       </c>
       <c r="L28" s="12" t="n">
         <f aca="false">E56</f>
-        <v>-0.0498126796585316</v>
+        <v>-0.300902664233209</v>
       </c>
       <c r="M28" s="12" t="n">
         <f aca="false">E57</f>
-        <v>-0.0191150997460902</v>
+        <v>-0.254969149404916</v>
       </c>
       <c r="N28" s="12" t="n">
         <f aca="false">E57</f>
-        <v>-0.0191150997460902</v>
+        <v>-0.254969149404916</v>
       </c>
       <c r="Q28" s="5" t="n">
         <f aca="false">IF(A19&lt;0,0,I28)</f>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="R28" s="5" t="n">
         <f aca="false">IF(B19&lt;0,0,J28)</f>
-        <v>0.0330686857057358</v>
+        <v>0.351023110175448</v>
       </c>
       <c r="S28" s="5" t="n">
         <f aca="false">IF(C19&lt;0,0,K28)</f>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="J29" s="11" t="n">
         <f aca="false">E58</f>
-        <v>-0.0146910307814731</v>
+        <v>0.167001376992702</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>0</v>
@@ -3307,11 +3307,11 @@
       </c>
       <c r="M29" s="11" t="n">
         <f aca="false">E60</f>
-        <v>0.0426737744072726</v>
+        <v>0.324905449234489</v>
       </c>
       <c r="N29" s="12" t="n">
         <f aca="false">E60</f>
-        <v>0.0426737744072726</v>
+        <v>0.324905449234489</v>
       </c>
       <c r="Q29" s="5" t="n">
         <f aca="false">IF(A20&lt;0,0,I29)</f>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="R29" s="5" t="n">
         <f aca="false">IF(B20&lt;0,0,J29)</f>
-        <v>-0.0146910307814731</v>
+        <v>0.167001376992702</v>
       </c>
       <c r="S29" s="5" t="n">
         <f aca="false">IF(C20&lt;0,0,K29)</f>
@@ -3375,15 +3375,15 @@
       </c>
       <c r="L30" s="11" t="n">
         <f aca="false">E59</f>
-        <v>0.0562326181612015</v>
+        <v>0.550288150456022</v>
       </c>
       <c r="M30" s="12" t="n">
         <f aca="false">E60</f>
-        <v>0.0426737744072726</v>
+        <v>0.324905449234489</v>
       </c>
       <c r="N30" s="12" t="n">
         <f aca="false">E60</f>
-        <v>0.0426737744072726</v>
+        <v>0.324905449234489</v>
       </c>
       <c r="Q30" s="5" t="n">
         <f aca="false">IF(A21&lt;0,0,I30)</f>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="T30" s="5" t="n">
         <f aca="false">IF(D21&lt;0,0,L30)</f>
-        <v>0.0562326181612015</v>
+        <v>0.550288150456022</v>
       </c>
       <c r="U30" s="5" t="n">
         <f aca="false">IF(E21&lt;0,0,M30)</f>
@@ -3438,11 +3438,11 @@
       </c>
       <c r="I31" s="11" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>0</v>
@@ -3509,25 +3509,25 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="11" t="n">
         <f aca="false">E62</f>
-        <v>-0.0699438888709005</v>
+        <v>-0.338939968904806</v>
       </c>
       <c r="M32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="11" t="n">
         <f aca="false">E63</f>
-        <v>0.049919248818131</v>
+        <v>0.466407750137834</v>
       </c>
       <c r="Q32" s="5" t="n">
         <f aca="false">IF(A23&lt;0,0,I32)</f>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="T32" s="5" t="n">
         <f aca="false">IF(D23&lt;0,0,L32)</f>
-        <v>-0.0699438888709005</v>
+        <v>-0.338939968904806</v>
       </c>
       <c r="U32" s="5" t="n">
         <f aca="false">IF(E23&lt;0,0,M32)</f>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="V32" s="5" t="n">
         <f aca="false">IF(F23&lt;0,0,N32)</f>
-        <v>0.049919248818131</v>
+        <v>0.466407750137834</v>
       </c>
       <c r="W32" s="13"/>
     </row>
@@ -3582,11 +3582,11 @@
       </c>
       <c r="I33" s="14" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="J33" s="14" t="n">
         <f aca="false">E61</f>
-        <v>-0.0178320153016612</v>
+        <v>-0.0229529676930111</v>
       </c>
       <c r="K33" s="14" t="n">
         <f aca="false">A86</f>
@@ -3890,6 +3890,15 @@
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+      <c r="V46" s="22"/>
+      <c r="W46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
@@ -3918,16 +3927,16 @@
         <v>0.00262993272951222</v>
       </c>
       <c r="K47" s="5" t="n">
-        <f aca="false">1/(1+EXP(-1*K44))</f>
-        <v>0.453228360515491</v>
+        <f aca="false">TANH(K44)</f>
+        <v>-0.185463686687083</v>
       </c>
       <c r="L47" s="5" t="n">
-        <f aca="false">1/(1+EXP(-1*L44))</f>
-        <v>0.515527888733896</v>
+        <f aca="false">TANH(L44)</f>
+        <v>0.0620517084632949</v>
       </c>
       <c r="M47" s="5" t="n">
-        <f aca="false">1/(1+EXP(-1*M44))</f>
-        <v>0.455556192726922</v>
+        <f aca="false">TANH(M44)</f>
+        <v>-0.176381636368834</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4016,16 +4025,16 @@
         <v>0</v>
       </c>
       <c r="K50" s="5" t="n">
-        <f aca="false">K47*(1-K47)</f>
-        <v>0.247812413739931</v>
+        <f aca="false">1-K47*K47</f>
+        <v>0.965603220920435</v>
       </c>
       <c r="L50" s="5" t="n">
-        <f aca="false">L47*(1-L47)</f>
-        <v>0.249758884671468</v>
+        <f aca="false">1-L47*L47</f>
+        <v>0.996149585476786</v>
       </c>
       <c r="M50" s="5" t="n">
-        <f aca="false">M47*(1-M47)</f>
-        <v>0.248024747995073</v>
+        <f aca="false">1-M47*M47</f>
+        <v>0.968889518351853</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4088,7 +4097,7 @@
       <c r="M52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K53" s="22" t="n">
+      <c r="K53" s="23" t="n">
         <v>0.32</v>
       </c>
       <c r="L53" s="5" t="n">
@@ -4113,22 +4122,22 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="n">
         <f aca="false">K$59*A44</f>
-        <v>-0.00657302265732036</v>
+        <v>0.0971704142739406</v>
       </c>
       <c r="B55" s="5" t="n">
         <f aca="false">L$59*B44</f>
-        <v>0.00293093068121346</v>
+        <v>-0.0692080842272607</v>
       </c>
       <c r="C55" s="5" t="n">
         <f aca="false">M$59*C44</f>
-        <v>0.0367107776818427</v>
-      </c>
-      <c r="E55" s="22" t="n">
+        <v>0.323060780128768</v>
+      </c>
+      <c r="E55" s="23" t="n">
         <f aca="false">SUM(A55:C55)</f>
-        <v>0.0330686857057358</v>
-      </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+        <v>0.351023110175448</v>
+      </c>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
       <c r="K55" s="4" t="s">
         <v>42</v>
       </c>
@@ -4138,74 +4147,74 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="n">
         <f aca="false">K$59*A45</f>
-        <v>0.000502254690387064</v>
+        <v>-0.00742493961763354</v>
       </c>
       <c r="B56" s="5" t="n">
         <f aca="false">L$59*B45</f>
-        <v>-0.00460620926414296</v>
+        <v>0.10876644772411</v>
       </c>
       <c r="C56" s="5" t="n">
         <f aca="false">M$59*C45</f>
-        <v>-0.0457087250847757</v>
-      </c>
-      <c r="E56" s="22" t="n">
+        <v>-0.402244172339686</v>
+      </c>
+      <c r="E56" s="23" t="n">
         <f aca="false">SUM(A56:C56)</f>
-        <v>-0.0498126796585316</v>
-      </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
+        <v>-0.300902664233209</v>
+      </c>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
       <c r="K56" s="5" t="n">
         <f aca="false">K47-K53</f>
-        <v>0.133228360515491</v>
+        <v>-0.505463686687083</v>
       </c>
       <c r="L56" s="5" t="n">
         <f aca="false">L47-L53</f>
-        <v>0.0655278887338959</v>
+        <v>-0.387948291536705</v>
       </c>
       <c r="M56" s="5" t="n">
         <f aca="false">M47-M53</f>
-        <v>-0.504443807273078</v>
+        <v>-1.13638163636883</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="n">
         <f aca="false">K$59*A46</f>
-        <v>0.0103550245428464</v>
+        <v>-0.153080565381074</v>
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">L$59*B46</f>
-        <v>-0.00485769474887244</v>
+        <v>0.114704776023941</v>
       </c>
       <c r="C57" s="5" t="n">
         <f aca="false">M$59*C46</f>
-        <v>-0.0246124295400642</v>
-      </c>
-      <c r="E57" s="22" t="n">
+        <v>-0.216593360047783</v>
+      </c>
+      <c r="E57" s="23" t="n">
         <f aca="false">SUM(A57:C57)</f>
-        <v>-0.0191150997460902</v>
-      </c>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+        <v>-0.254969149404916</v>
+      </c>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="n">
         <f aca="false">K$59*A47</f>
-        <v>-0.00943376157440863</v>
+        <v>0.139461335847665</v>
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">L$59*B47</f>
-        <v>-0.00227700237819075</v>
+        <v>0.0537668711804043</v>
       </c>
       <c r="C58" s="5" t="n">
         <f aca="false">M$59*C47</f>
-        <v>-0.00298026682887373</v>
-      </c>
-      <c r="E58" s="22" t="n">
+        <v>-0.0262268300353671</v>
+      </c>
+      <c r="E58" s="23" t="n">
         <f aca="false">SUM(A58:C58)</f>
-        <v>-0.0146910307814731</v>
-      </c>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
+        <v>0.167001376992702</v>
+      </c>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
       <c r="K58" s="2" t="s">
         <v>43</v>
       </c>
@@ -4215,83 +4224,83 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="n">
         <f aca="false">K$59*A48</f>
-        <v>-0.00394017946537445</v>
+        <v>0.0582485244498145</v>
       </c>
       <c r="B59" s="5" t="n">
         <f aca="false">L$59*B48</f>
-        <v>0.00115665102060833</v>
+        <v>-0.0273120076735032</v>
       </c>
       <c r="C59" s="5" t="n">
         <f aca="false">M$59*C48</f>
-        <v>0.0590161466059677</v>
-      </c>
-      <c r="E59" s="22" t="n">
+        <v>0.519351633679711</v>
+      </c>
+      <c r="E59" s="23" t="n">
         <f aca="false">SUM(A59:C59)</f>
-        <v>0.0562326181612015</v>
-      </c>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
+        <v>0.550288150456022</v>
+      </c>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
       <c r="K59" s="5" t="n">
         <f aca="false">K56*K50</f>
-        <v>0.0330156415979575</v>
+        <v>-0.488077363923366</v>
       </c>
       <c r="L59" s="5" t="n">
         <f aca="false">L56*L50</f>
-        <v>0.0163661724050539</v>
+        <v>-0.386454529800716</v>
       </c>
       <c r="M59" s="5" t="n">
         <f aca="false">M56*M50</f>
-        <v>-0.125114548176581</v>
+        <v>-1.10102825632529</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="n">
         <f aca="false">K$59*A49</f>
-        <v>-0.00600692610798789</v>
+        <v>0.0888016866602571</v>
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">L$59*B49</f>
-        <v>0.00593259736062791</v>
+        <v>-0.140086458015709</v>
       </c>
       <c r="C60" s="5" t="n">
         <f aca="false">M$59*C49</f>
-        <v>0.0427481031546326</v>
-      </c>
-      <c r="E60" s="22" t="n">
+        <v>0.37619022058994</v>
+      </c>
+      <c r="E60" s="23" t="n">
         <f aca="false">SUM(A60:C60)</f>
-        <v>0.0426737744072726</v>
-      </c>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="I60" s="23" t="s">
+        <v>0.324905449234489</v>
+      </c>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="I60" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J60" s="23"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
+      <c r="J60" s="24"/>
+      <c r="K60" s="24"/>
+      <c r="L60" s="24"/>
+      <c r="M60" s="24"/>
+      <c r="N60" s="24"/>
+      <c r="O60" s="24"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="n">
         <f aca="false">K$59*A50</f>
-        <v>-0.00102712173075847</v>
+        <v>0.0151841624912723</v>
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">L$59*B50</f>
-        <v>-0.00338592794178138</v>
+        <v>0.0799519373434048</v>
       </c>
       <c r="C61" s="5" t="n">
         <f aca="false">M$59*C50</f>
-        <v>-0.0134189656291214</v>
-      </c>
-      <c r="E61" s="22" t="n">
+        <v>-0.118089067527688</v>
+      </c>
+      <c r="E61" s="23" t="n">
         <f aca="false">SUM(A61:C61)</f>
-        <v>-0.0178320153016612</v>
-      </c>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
+        <v>-0.0229529676930111</v>
+      </c>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
       <c r="K61" s="5" t="n">
         <v>0</v>
       </c>
@@ -4305,43 +4314,43 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="n">
         <f aca="false">K$59*A51</f>
-        <v>-0.00716326670362306</v>
+        <v>0.105896119553244</v>
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">L$59*B51</f>
-        <v>-0.00332098174882929</v>
+        <v>0.0784183624892199</v>
       </c>
       <c r="C62" s="5" t="n">
         <f aca="false">M$59*C51</f>
-        <v>-0.0594596404184482</v>
-      </c>
-      <c r="D62" s="24"/>
-      <c r="E62" s="22" t="n">
+        <v>-0.52325445094727</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="23" t="n">
         <f aca="false">SUM(A62:C62)</f>
-        <v>-0.0699438888709005</v>
-      </c>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
+        <v>-0.338939968904806</v>
+      </c>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="n">
         <f aca="false">K$59*A52</f>
-        <v>-0.00683087492545076</v>
+        <v>0.100982300071687</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">L$59*B52</f>
-        <v>0.00413365384470549</v>
+        <v>-0.0976079936944378</v>
       </c>
       <c r="C63" s="5" t="n">
         <f aca="false">M$59*C52</f>
-        <v>0.0526164698988763</v>
-      </c>
-      <c r="E63" s="22" t="n">
+        <v>0.463033443760584</v>
+      </c>
+      <c r="E63" s="23" t="n">
         <f aca="false">SUM(A63:C63)</f>
-        <v>0.049919248818131</v>
-      </c>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
+        <v>0.466407750137834</v>
+      </c>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="18"/>
@@ -4361,41 +4370,41 @@
       <c r="G65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="22" t="n">
+      <c r="A66" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E44+$O$43*$Q$43*A44</f>
-        <v>5.13457934020712E-005</v>
-      </c>
-      <c r="B66" s="22" t="n">
+        <v>-0.000790478470155304</v>
+      </c>
+      <c r="B66" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E44+$O$43*$Q$43*B44</f>
-        <v>2.82303515810986E-005</v>
-      </c>
-      <c r="C66" s="22" t="n">
+        <v>-0.00062252534344264</v>
+      </c>
+      <c r="C66" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E44+$O$43*$Q$43*C44</f>
-        <v>-0.000205056368964151</v>
+        <v>-0.00178164217985202</v>
       </c>
       <c r="E66" s="9" t="n">
         <f aca="false">A44-A66</f>
-        <v>-0.199139485208115</v>
+        <v>-0.198297660944558</v>
       </c>
       <c r="F66" s="9" t="n">
         <f aca="false">B44-B66</f>
-        <v>0.179056445568635</v>
+        <v>0.179707201263659</v>
       </c>
       <c r="G66" s="9" t="n">
         <f aca="false">C44-C66</f>
-        <v>-0.293212281717337</v>
+        <v>-0.291635695906449</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="n">
+      <c r="A67" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E45+$O$43*$Q$43*A45</f>
         <v>1.52126285020654E-007</v>
       </c>
-      <c r="B67" s="22" t="n">
+      <c r="B67" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E45+$O$43*$Q$43*B45</f>
         <v>-2.81446947407236E-006</v>
       </c>
-      <c r="C67" s="22" t="n">
+      <c r="C67" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E45+$O$43*$Q$43*C45</f>
         <v>3.65335013001561E-006</v>
       </c>
@@ -4413,15 +4422,15 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="22" t="n">
+      <c r="A68" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E46+$O$43*$Q$43*A46</f>
         <v>3.13639960990097E-006</v>
       </c>
-      <c r="B68" s="22" t="n">
+      <c r="B68" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E46+$O$43*$Q$43*B46</f>
         <v>-2.96813123352677E-006</v>
       </c>
-      <c r="C68" s="22" t="n">
+      <c r="C68" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E46+$O$43*$Q$43*C46</f>
         <v>1.96719165746635E-006</v>
       </c>
@@ -4439,67 +4448,67 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="n">
+      <c r="A69" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E47+$O$43*$Q$43*A47</f>
-        <v>3.35942763504842E-005</v>
-      </c>
-      <c r="B69" s="22" t="n">
+        <v>-0.00054172979692706</v>
+      </c>
+      <c r="B69" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E47+$O$43*$Q$43*B47</f>
-        <v>1.66781429888967E-005</v>
-      </c>
-      <c r="C69" s="22" t="n">
+        <v>-0.000428064819856459</v>
+      </c>
+      <c r="C69" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E47+$O$43*$Q$43*C47</f>
-        <v>-0.00013789723671808</v>
+        <v>-0.00121537600498094</v>
       </c>
       <c r="E69" s="9" t="n">
         <f aca="false">A47-A69</f>
-        <v>-0.285769721693975</v>
+        <v>-0.285194397620698</v>
       </c>
       <c r="F69" s="9" t="n">
         <f aca="false">B47-B69</f>
-        <v>-0.139145261286083</v>
+        <v>-0.138700518323238</v>
       </c>
       <c r="G69" s="9" t="n">
         <f aca="false">C47-C69</f>
-        <v>0.0239582032867189</v>
+        <v>0.0250356820549817</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="22" t="n">
+      <c r="A70" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E48+$O$43*$Q$43*A48</f>
-        <v>7.1486836026506E-005</v>
-      </c>
-      <c r="B70" s="22" t="n">
+        <v>-0.0010756414778984</v>
+      </c>
+      <c r="B70" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E48+$O$43*$Q$43*B48</f>
-        <v>3.67350416374171E-005</v>
-      </c>
-      <c r="C70" s="22" t="n">
+        <v>-0.000850029946645355</v>
+      </c>
+      <c r="C70" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E48+$O$43*$Q$43*C48</f>
-        <v>-0.000280142736115372</v>
+        <v>-0.00242850825763074</v>
       </c>
       <c r="E70" s="9" t="n">
         <f aca="false">A48-A70</f>
-        <v>-0.119414297536341</v>
+        <v>-0.118267169222416</v>
       </c>
       <c r="F70" s="9" t="n">
         <f aca="false">B48-B70</f>
-        <v>0.0706365410293852</v>
+        <v>0.071523306017668</v>
       </c>
       <c r="G70" s="9" t="n">
         <f aca="false">C48-C70</f>
-        <v>-0.471416773937995</v>
+        <v>-0.469268408416479</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="22" t="n">
+      <c r="A71" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E49+$O$43*$Q$43*A49</f>
         <v>-1.8194182566967E-006</v>
       </c>
-      <c r="B71" s="22" t="n">
+      <c r="B71" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E49+$O$43*$Q$43*B49</f>
         <v>3.62491437447886E-006</v>
       </c>
-      <c r="C71" s="22" t="n">
+      <c r="C71" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E49+$O$43*$Q$43*C49</f>
         <v>-3.41671722254872E-006</v>
       </c>
@@ -4517,15 +4526,15 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="22" t="n">
+      <c r="A72" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E50+$O$43*$Q$43*A50</f>
         <v>-3.11101550975768E-007</v>
       </c>
-      <c r="B72" s="22" t="n">
+      <c r="B72" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E50+$O$43*$Q$43*B50</f>
         <v>-2.06885755446142E-006</v>
       </c>
-      <c r="C72" s="22" t="n">
+      <c r="C72" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E50+$O$43*$Q$43*C50</f>
         <v>1.07253439545515E-006</v>
       </c>
@@ -4543,59 +4552,59 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="22" t="n">
+      <c r="A73" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E51+$O$43*$Q$43*A51</f>
-        <v>5.86752262923846E-005</v>
-      </c>
-      <c r="B73" s="22" t="n">
+        <v>-0.000901652737858782</v>
+      </c>
+      <c r="B73" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E51+$O$43*$Q$43*B51</f>
-        <v>2.81322226609722E-005</v>
-      </c>
-      <c r="C73" s="22" t="n">
+        <v>-0.000714230428091171</v>
+      </c>
+      <c r="C73" s="23" t="n">
         <f aca="false">$O$43*(M$59+M$61*$P$43)*$E51+$O$43*$Q$43*C51</f>
-        <v>-0.000225822544639942</v>
+        <v>-0.00202434452555975</v>
       </c>
       <c r="E73" s="9" t="n">
         <f aca="false">A51-A73</f>
-        <v>-0.217024524045847</v>
+        <v>-0.216064196081696</v>
       </c>
       <c r="F73" s="9" t="n">
         <f aca="false">B51-B73</f>
-        <v>-0.202945568666369</v>
+        <v>-0.202203206015617</v>
       </c>
       <c r="G73" s="9" t="n">
         <f aca="false">C51-C73</f>
-        <v>0.475467441405218</v>
+        <v>0.477265963386138</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="22" t="n">
+      <c r="A74" s="23" t="n">
         <f aca="false">$O$43*(K$59+K$61*$P$43)*$E52+$O$43*$Q$43*A52</f>
-        <v>8.99548720441683E-005</v>
-      </c>
-      <c r="B74" s="22" t="n">
+        <v>-0.00136247749224827</v>
+      </c>
+      <c r="B74" s="23" t="n">
         <f aca="false">$O$43*(L$59+L$61*$P$43)*$E52+$O$43*$Q$43*B52</f>
-        <v>4.81428432870336E-005</v>
-      </c>
-      <c r="C74" s="22" t="n">
-        <f aca="false">$O$43*(M$59+M$61*$P$43)*$E52</f>
-        <v>-0.000348729338313975</v>
+        <v>-0.00107463143825478</v>
+      </c>
+      <c r="C74" s="23" t="n">
+        <f aca="false">$O$43*(M$59+M$61*$P$43)*$E52+$O$43*$Q$43*C52</f>
+        <v>-0.00307308003422311</v>
       </c>
       <c r="E74" s="9" t="n">
         <f aca="false">A52-A74</f>
-        <v>-0.206988097535228</v>
+        <v>-0.205535665170936</v>
       </c>
       <c r="F74" s="9" t="n">
         <f aca="false">B52-B74</f>
-        <v>0.252524892708325</v>
+        <v>0.253647666989867</v>
       </c>
       <c r="G74" s="9" t="n">
         <f aca="false">C52-C74</f>
-        <v>-0.420197647287814</v>
+        <v>-0.417473296591905</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="46">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="Z1:AE1"/>
@@ -4623,6 +4632,7 @@
     <mergeCell ref="P41:P42"/>
     <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="K46:M46"/>
+    <mergeCell ref="O46:W46"/>
     <mergeCell ref="K49:M49"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="A54:C54"/>

</xml_diff>